<commit_message>
Added various standard-named components to the Schematic header library Updated Switch Library component names spreadsheet Split Wings 3D Library Info spreadsheet into seperate files for each tab Added the individual 3D Library spreadsheet files to repo Removed Wings 3D Library Info spreadsheet Added 0603 LED components to 3D Library
</commit_message>
<xml_diff>
--- a/PCB/Switch_Library_Component_Names.xlsx
+++ b/PCB/Switch_Library_Component_Names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>SW_PUSH_1P1T_OFF-ON</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>SW_ROCKER_ON-OFF-ON</t>
+  </si>
+  <si>
+    <t>SW_FSM4JH_PTH</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A9"/>
+  <dimension ref="A2:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -458,6 +461,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <headerFooter>

</xml_diff>